<commit_message>
add skel rows to req
</commit_message>
<xml_diff>
--- a/part1/requirements.xlsx
+++ b/part1/requirements.xlsx
@@ -21,6 +21,23 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Desc</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -336,12 +353,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>